<commit_message>
Import kyc docs now uses Investing Entity and Pan/Tax Id
</commit_message>
<xml_diff>
--- a/public/sample_uploads/investor_kycs.xlsx
+++ b/public/sample_uploads/investor_kycs.xlsx
@@ -1116,8 +1116,8 @@
   </sheetPr>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1:V5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1209,7 +1209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>